<commit_message>
Comparación y resultados estadísticos
</commit_message>
<xml_diff>
--- a/Estadística/Cuantitativo/Analisis cuantitativo.xlsx
+++ b/Estadística/Cuantitativo/Analisis cuantitativo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmvg2\Documents\Repositorio_Pulsos\Pulsos_Binaurales\Estadística\Cuantitativo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF2A4FC-FBB1-4E1F-B060-43B594B401BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829F90C8-EC6A-44D0-885F-6A3DA73F5956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="7" xr2:uid="{EF9B71AE-CFE6-45D1-BA90-996948001BCF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EF9B71AE-CFE6-45D1-BA90-996948001BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Pruebas aritmeticas" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="ErrorTotal" sheetId="8" r:id="rId7"/>
     <sheet name="Error" sheetId="6" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pruebas aritmeticas'!$A$1:$E$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -65,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="61">
   <si>
     <t>Sujeto</t>
   </si>
@@ -244,10 +247,10 @@
     <t>Diferencia</t>
   </si>
   <si>
-    <t>Sin Pulsos</t>
+    <t>Ruido Rosa</t>
   </si>
   <si>
-    <t>Con Pulsos</t>
+    <t>Sí</t>
   </si>
 </sst>
 </file>
@@ -580,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -701,6 +704,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -911,58 +920,60 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="38100" cap="rnd" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Pruebas aritmeticas'!$K$3:$K$18</c:f>
+              <c:f>'Pruebas aritmeticas'!$L$3:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-8</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
@@ -970,57 +981,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Pruebas aritmeticas'!$M$3:$M$18</c:f>
+              <c:f>'Pruebas aritmeticas'!$N$3:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-1.8627318674216511</c:v>
+                  <c:v>-1.6906216295848977</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.3180108973035372</c:v>
+                  <c:v>-1.096803562093513</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.0099901692495805</c:v>
+                  <c:v>-0.74785859476330196</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.77642176114792794</c:v>
+                  <c:v>-0.47278912099226744</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.57913216225555586</c:v>
+                  <c:v>-0.22988411757923208</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.40225006532172536</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.23720210932878771</c:v>
+                  <c:v>0.22988411757923222</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-7.8412412733112211E-2</c:v>
+                  <c:v>0.47278912099226728</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.8412412733112211E-2</c:v>
+                  <c:v>0.74785859476330196</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23720210932878771</c:v>
+                  <c:v>1.096803562093513</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.40225006532172536</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.57913216225555586</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.77642176114792794</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.0099901692495805</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.3180108973035372</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.8627318674216511</c:v>
+                  <c:v>1.6906216295848984</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1497,8 +1493,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.15695729563413124"/>
-                  <c:y val="-1.2337805099154995E-2"/>
+                  <c:x val="-2.8061964206975747E-2"/>
+                  <c:y val="0.26035572256551515"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1530,48 +1526,48 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Pruebas aritmeticas'!$K$14:$K$18</c:f>
+              <c:f>'Pruebas aritmeticas'!$L$21:$L$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Pruebas aritmeticas'!$M$14:$M$18</c:f>
+              <c:f>'Pruebas aritmeticas'!$N$21:$N$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.57913216225555586</c:v>
+                  <c:v>-1.6906216295848977</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77642176114792794</c:v>
+                  <c:v>-1.096803562093513</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0099901692495805</c:v>
+                  <c:v>-0.74785859476330196</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3180108973035372</c:v>
+                  <c:v>-0.47278912099226744</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8627318674216511</c:v>
+                  <c:v>-0.22988411757923208</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7887,16 +7883,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>379236</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>114653</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>301359</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66729</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>87976</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>50209</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>10099</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>2285</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7925,13 +7921,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>377406</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>167736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>86146</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>145226</xdr:rowOff>
@@ -8430,841 +8426,842 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66B3B4F-3D75-4B95-86A7-DCDAAB7758F6}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView zoomScale="106" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="27.6328125" customWidth="1"/>
+    <col min="7" max="7" width="27.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>53</v>
       </c>
-      <c r="K1">
-        <f>COUNT(B2:B350)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L1">
+        <f>COUNTIF(B1:B50,"No")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <f>C2-B2</f>
+      <c r="E2">
+        <f>D2-C2</f>
         <v>-1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>54</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>55</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>56</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D17" si="0">C3-B3</f>
+      <c r="E3">
+        <f t="shared" ref="E3:E17" si="0">D3-C3</f>
         <v>4</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="21"/>
+      <c r="H3" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>1</v>
       </c>
-      <c r="K3" s="13" cm="1">
-        <f t="array" ref="K3:K18">_xlfn._xlws.SORT(D2:D17,,1)</f>
-        <v>-8</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L18" si="1">(J3-0.5)/$K$1</f>
-        <v>3.125E-2</v>
+      <c r="L3" s="13" cm="1">
+        <f t="array" ref="L3:L13">_xlfn._xlws.SORT(E2:E12,,1)</f>
+        <v>-3</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M18" si="2">_xlfn.NORM.S.INV(L3)</f>
-        <v>-1.8627318674216511</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <f t="shared" ref="M3:M18" si="1">(K3-0.5)/$L$1</f>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N18" si="2">_xlfn.NORM.S.INV(M3)</f>
+        <v>-1.6906216295848977</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>35</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>-0.54545454545454541</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.81818181818181823</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2</v>
       </c>
-      <c r="K4" s="23">
-        <v>-3</v>
-      </c>
-      <c r="L4">
+      <c r="L4" s="23">
+        <v>-2</v>
+      </c>
+      <c r="M4">
         <f t="shared" si="1"/>
-        <v>9.375E-2</v>
-      </c>
-      <c r="M4">
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="N4">
         <f t="shared" si="2"/>
-        <v>-1.3180108973035372</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>-1.096803562093513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
         <v>-3</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>-2</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>36</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>5.6727272727272728</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>12.563636363636364</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>3</v>
       </c>
-      <c r="K5" s="13">
-        <v>-2</v>
-      </c>
-      <c r="L5">
+      <c r="L5" s="13">
+        <v>-1</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="1"/>
-        <v>0.15625</v>
-      </c>
-      <c r="M5">
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="2"/>
-        <v>-1.0099901692495805</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>-0.74785859476330196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
         <v>-2</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>-1</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>37</v>
-      </c>
-      <c r="G6">
-        <v>11</v>
       </c>
       <c r="H6">
         <v>11</v>
       </c>
-      <c r="J6">
+      <c r="I6">
+        <v>11</v>
+      </c>
+      <c r="K6">
         <v>4</v>
       </c>
-      <c r="K6" s="13">
-        <v>-2</v>
-      </c>
-      <c r="L6">
+      <c r="L6" s="13">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="1"/>
-        <v>0.21875</v>
-      </c>
-      <c r="M6">
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="2"/>
-        <v>-0.77642176114792794</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>-0.47278912099226744</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
         <v>-3</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>-6</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>38</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.54380733575410534</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>5</v>
       </c>
-      <c r="K7" s="23">
-        <v>-1</v>
-      </c>
-      <c r="L7">
+      <c r="L7" s="23">
+        <v>1</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="1"/>
-        <v>0.28125</v>
-      </c>
-      <c r="M7">
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="N7">
         <f t="shared" si="2"/>
-        <v>-0.57913216225555586</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>-0.22988411757923208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>6</v>
       </c>
-      <c r="K8" s="23">
+      <c r="L8" s="23">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L8">
-        <f t="shared" si="1"/>
-        <v>0.34375</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="2"/>
-        <v>-0.40225006532172536</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
         <v>-1</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>-3</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>40</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>10</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>7</v>
       </c>
-      <c r="K9" s="13">
+      <c r="L9" s="13">
         <v>1</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="1"/>
-        <v>0.40625</v>
-      </c>
-      <c r="M9">
+        <v>0.59090909090909094</v>
+      </c>
+      <c r="N9">
         <f t="shared" si="2"/>
-        <v>-0.23720210932878771</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+        <v>0.22988411757923222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="G10" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="22">
+      <c r="H10" s="22">
         <v>-1.5030090301053793</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>8</v>
       </c>
-      <c r="K10" s="29">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="1"/>
-        <v>0.46875</v>
+      <c r="L10" s="29">
+        <v>2</v>
       </c>
       <c r="M10">
+        <f>(K10-0.5)/$L$1</f>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="2"/>
-        <v>-7.8412412733112211E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <v>0.47278912099226728</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
         <v>-4</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>4</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="G11" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="22">
+      <c r="H11" s="22">
         <v>8.1870954407484459E-2</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>9</v>
       </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
       <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="1"/>
-        <v>0.53125</v>
-      </c>
-      <c r="M11">
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="2"/>
-        <v>7.8412412733112211E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+        <v>0.74785859476330196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>3</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="G12" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="22">
+      <c r="H12" s="22">
         <v>1.812461122811676</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>10</v>
       </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
       <c r="L12">
+        <v>4</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="1"/>
-        <v>0.59375</v>
-      </c>
-      <c r="M12">
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="2"/>
-        <v>0.23720210932878771</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+        <v>1.096803562093513</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <f t="shared" si="0"/>
         <v>-8</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>44</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.16374190881496892</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>11</v>
       </c>
-      <c r="K13" s="28">
-        <v>2</v>
-      </c>
-      <c r="L13">
+      <c r="L13" s="28">
+        <v>8</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="1"/>
-        <v>0.65625</v>
-      </c>
-      <c r="M13">
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="2"/>
-        <v>0.40225006532172536</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>1.6906216295848984</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>10</v>
+      <c r="B14" t="s">
+        <v>60</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="G14" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="20">
+      <c r="H14" s="20">
         <v>2.2281388519862744</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="J14">
-        <v>12</v>
-      </c>
-      <c r="K14">
-        <v>3</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="1"/>
-        <v>0.71875</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
-        <v>0.57913216225555586</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15">
         <v>8</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>6</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="J15">
-        <v>13</v>
-      </c>
-      <c r="K15">
-        <v>3</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="1"/>
-        <v>0.78125</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
-        <v>0.77642176114792794</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16">
         <v>5</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>11</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16">
-        <v>14</v>
-      </c>
-      <c r="K16">
-        <v>4</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="1"/>
-        <v>0.84375</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
-        <v>1.0099901692495805</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17">
         <v>3</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>6</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J17">
-        <v>15</v>
-      </c>
-      <c r="K17">
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G19" s="43"/>
+      <c r="H19" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G20" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="41">
+        <v>7.2</v>
+      </c>
+      <c r="I20" s="47">
+        <v>7</v>
+      </c>
+      <c r="K20" t="s">
+        <v>53</v>
+      </c>
+      <c r="L20">
+        <f>COUNTIF(B1:B50,"Sí")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G21" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="41">
+        <v>9.7000000000000028</v>
+      </c>
+      <c r="I21" s="41">
+        <v>13</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21" cm="1">
+        <f t="array" ref="L21:L25">_xlfn._xlws.SORT(E13:E17,,1)</f>
+        <v>-8</v>
+      </c>
+      <c r="M21">
+        <f>(K21-0.5)/$L$1</f>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="N21">
+        <f>_xlfn.NORM.S.INV(M21)</f>
+        <v>-1.6906216295848977</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G22" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="41">
+        <v>5</v>
+      </c>
+      <c r="I22" s="41">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>-2</v>
+      </c>
+      <c r="M22">
+        <f>(K22-0.5)/$L$1</f>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="N22">
+        <f>_xlfn.NORM.S.INV(M22)</f>
+        <v>-1.096803562093513</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G23" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="41">
+        <v>-0.24489231153834698</v>
+      </c>
+      <c r="I23" s="41"/>
+      <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>(K23-0.5)/$L$1</f>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="N23">
+        <f>_xlfn.NORM.S.INV(M23)</f>
+        <v>-0.74785859476330196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G24" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" s="41">
+        <v>0</v>
+      </c>
+      <c r="I24" s="41"/>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <f>(K24-0.5)/$L$1</f>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="N24">
+        <f>_xlfn.NORM.S.INV(M24)</f>
+        <v>-0.47278912099226744</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G25" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="41">
+        <v>4</v>
+      </c>
+      <c r="I25" s="41"/>
+      <c r="K25">
+        <v>5</v>
+      </c>
+      <c r="L25" s="24">
         <v>6</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="1"/>
-        <v>0.90625</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="2"/>
-        <v>1.3180108973035372</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F18" s="43"/>
-      <c r="G18" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18">
-        <v>16</v>
-      </c>
-      <c r="K18" s="24">
-        <v>8</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="1"/>
-        <v>0.96875</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="2"/>
-        <v>1.8627318674216511</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F19" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="41">
-        <v>1.875</v>
-      </c>
-      <c r="H19" s="41">
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F20" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="41">
-        <v>20.116666666666667</v>
-      </c>
-      <c r="H20" s="41">
-        <v>20.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F21" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="41">
-        <v>16</v>
-      </c>
-      <c r="H21" s="41">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F22" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="41">
-        <v>0.65334116248127649</v>
-      </c>
-      <c r="H22" s="41"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F23" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="41">
-        <v>0</v>
-      </c>
-      <c r="H23" s="41"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F24" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="41">
-        <v>15</v>
-      </c>
-      <c r="H24" s="41"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F25" s="41" t="s">
+      <c r="M25">
+        <f>(K25-0.5)/$L$1</f>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="N25">
+        <f>_xlfn.NORM.S.INV(M25)</f>
+        <v>-0.22988411757923208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G26" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="41">
-        <v>-0.93154097872359987</v>
-      </c>
-      <c r="H25" s="41"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F26" s="41" t="s">
+      <c r="H26" s="46">
+        <v>8.4215192106651904E-2</v>
+      </c>
+      <c r="I26" s="41"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G27" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="41">
-        <v>0.18316278383292367</v>
-      </c>
-      <c r="H26" s="41"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F27" s="41" t="s">
+      <c r="H27" s="46">
+        <v>0.46846587804078005</v>
+      </c>
+      <c r="I27" s="41"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G28" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G27" s="41">
-        <v>1.7530503556925723</v>
-      </c>
-      <c r="H27" s="41"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F28" s="41" t="s">
+      <c r="H28" s="46">
+        <v>2.1318467863266499</v>
+      </c>
+      <c r="I28" s="41"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G29" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="41">
-        <v>0.36632556766584734</v>
-      </c>
-      <c r="H28" s="41"/>
-    </row>
-    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F29" s="42" t="s">
+      <c r="H29" s="41">
+        <v>0.9369317560815601</v>
+      </c>
+      <c r="I29" s="41"/>
+    </row>
+    <row r="30" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G30" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="G29" s="42">
-        <v>2.1314495455597742</v>
-      </c>
-      <c r="H29" s="42"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="F31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F33" s="43"/>
-      <c r="G33" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="H33" s="43" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F34" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="41">
-        <v>7.2</v>
-      </c>
-      <c r="H34" s="41">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F35" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="G35" s="41">
-        <v>9.7000000000000028</v>
-      </c>
-      <c r="H35" s="41">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F36" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="G36" s="41">
-        <v>5</v>
-      </c>
-      <c r="H36" s="41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F37" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" s="41">
-        <v>-0.24489231153834698</v>
-      </c>
-      <c r="H37" s="41"/>
-    </row>
-    <row r="38" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F38" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="G38" s="41">
-        <v>0</v>
-      </c>
-      <c r="H38" s="41"/>
-    </row>
-    <row r="39" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F39" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="G39" s="41">
-        <v>4</v>
-      </c>
-      <c r="H39" s="41"/>
-    </row>
-    <row r="40" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F40" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G40" s="41">
-        <v>8.4215192106651904E-2</v>
-      </c>
-      <c r="H40" s="41"/>
-    </row>
-    <row r="41" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F41" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="G41" s="41">
-        <v>0.46846587804078005</v>
-      </c>
-      <c r="H41" s="41"/>
-    </row>
-    <row r="42" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F42" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="G42" s="41">
-        <v>2.1318467863266499</v>
-      </c>
-      <c r="H42" s="41"/>
-    </row>
-    <row r="43" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F43" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" s="41">
-        <v>0.9369317560815601</v>
-      </c>
-      <c r="H43" s="41"/>
-    </row>
-    <row r="44" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F44" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="G44" s="42">
+      <c r="H30" s="42">
         <v>2.7764451051977934</v>
       </c>
-      <c r="H44" s="42"/>
+      <c r="I30" s="42"/>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G40" s="45"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+    </row>
+    <row r="43" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+    </row>
+    <row r="44" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K4:K18">
-    <sortCondition ref="K3:K18"/>
+  <autoFilter ref="A1:E17" xr:uid="{B66B3B4F-3D75-4B95-86A7-DCDAAB7758F6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L4:L18">
+    <sortCondition ref="L3:L18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10163,8 +10160,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="102" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView zoomScale="102" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11184,7 +11181,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>

</xml_diff>